<commit_message>
more training data and reduction of the features
</commit_message>
<xml_diff>
--- a/BantSpirit/Training_set_BantSpirit/Features.xlsx
+++ b/BantSpirit/Training_set_BantSpirit/Features.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t xml:space="preserve"> name_of_the_card</t>
   </si>
@@ -39,12 +39,6 @@
     <t>Need_G</t>
   </si>
   <si>
-    <t>power</t>
-  </si>
-  <si>
-    <t>Toughness</t>
-  </si>
-  <si>
     <t>Need_generic</t>
   </si>
   <si>
@@ -133,9 +127,6 @@
   </si>
   <si>
     <t>geist_of_saint_traft</t>
-  </si>
-  <si>
-    <t>produces_colorless</t>
   </si>
   <si>
     <t>Is_lord</t>
@@ -477,26 +468,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="6.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" customWidth="1"/>
+    <col min="13" max="13" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -510,136 +500,109 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" t="s">
-        <v>40</v>
-      </c>
-      <c r="N1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -674,19 +637,10 @@
       <c r="L4">
         <v>0</v>
       </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -721,19 +675,10 @@
       <c r="L5">
         <v>0</v>
       </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -768,19 +713,10 @@
       <c r="L6">
         <v>0</v>
       </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -815,19 +751,10 @@
       <c r="L7">
         <v>0</v>
       </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -862,19 +789,10 @@
       <c r="L8">
         <v>0</v>
       </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>7</v>
@@ -909,19 +827,10 @@
       <c r="L9">
         <v>0</v>
       </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>8</v>
@@ -956,19 +865,10 @@
       <c r="L10">
         <v>0</v>
       </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>9</v>
@@ -989,7 +889,7 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -1003,19 +903,10 @@
       <c r="L11">
         <v>0</v>
       </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B12">
         <v>10</v>
@@ -1036,7 +927,7 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -1050,19 +941,10 @@
       <c r="L12">
         <v>0</v>
       </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B13">
         <v>11</v>
@@ -1097,19 +979,10 @@
       <c r="L13">
         <v>0</v>
       </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14">
         <v>12</v>
@@ -1144,19 +1017,10 @@
       <c r="L14">
         <v>0</v>
       </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B15">
         <v>13</v>
@@ -1191,19 +1055,10 @@
       <c r="L15">
         <v>0</v>
       </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B16">
         <v>14</v>
@@ -1233,24 +1088,15 @@
         <v>0</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16">
-        <v>1</v>
-      </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B17">
         <v>15</v>
@@ -1271,10 +1117,10 @@
         <v>0</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17">
         <v>0</v>
@@ -1285,19 +1131,10 @@
       <c r="L17">
         <v>0</v>
       </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B18">
         <v>16</v>
@@ -1324,27 +1161,18 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18">
-        <v>0</v>
-      </c>
-      <c r="O18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B19">
         <v>17</v>
@@ -1368,10 +1196,10 @@
         <v>0</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -1379,19 +1207,10 @@
       <c r="L19">
         <v>0</v>
       </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19">
-        <v>1</v>
-      </c>
-      <c r="O19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B20">
         <v>18</v>
@@ -1415,30 +1234,21 @@
         <v>0</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20">
-        <v>1</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20">
-        <v>2</v>
-      </c>
-      <c r="O20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B21">
         <v>19</v>
@@ -1459,33 +1269,24 @@
         <v>0</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21">
         <v>0</v>
       </c>
       <c r="K21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L21">
-        <v>1</v>
-      </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
-      <c r="N21">
-        <v>2</v>
-      </c>
-      <c r="O21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B22">
         <v>20</v>
@@ -1509,30 +1310,21 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22">
-        <v>1</v>
-      </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-      <c r="N22">
-        <v>0</v>
-      </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B23">
         <v>21</v>
@@ -1556,30 +1348,21 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23">
         <v>1</v>
       </c>
-      <c r="M23">
-        <v>1</v>
-      </c>
-      <c r="N23">
-        <v>1</v>
-      </c>
-      <c r="O23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B24">
         <v>22</v>
@@ -1600,33 +1383,24 @@
         <v>0</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24">
         <v>1</v>
       </c>
       <c r="J24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L24">
-        <v>1</v>
-      </c>
-      <c r="M24">
-        <v>0</v>
-      </c>
-      <c r="N24">
-        <v>2</v>
-      </c>
-      <c r="O24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B25">
         <v>23</v>
@@ -1647,33 +1421,24 @@
         <v>0</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25">
         <v>1</v>
       </c>
       <c r="J25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L25">
         <v>1</v>
       </c>
-      <c r="M25">
-        <v>1</v>
-      </c>
-      <c r="N25">
-        <v>2</v>
-      </c>
-      <c r="O25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B26">
         <v>24</v>
@@ -1694,33 +1459,24 @@
         <v>0</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26">
         <v>1</v>
       </c>
       <c r="J26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L26">
-        <v>1</v>
-      </c>
-      <c r="M26">
-        <v>0</v>
-      </c>
-      <c r="N26">
-        <v>2</v>
-      </c>
-      <c r="O26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B27">
         <v>25</v>
@@ -1747,21 +1503,12 @@
         <v>0</v>
       </c>
       <c r="J27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L27">
-        <v>3</v>
-      </c>
-      <c r="M27">
-        <v>0</v>
-      </c>
-      <c r="N27">
-        <v>0</v>
-      </c>
-      <c r="O27">
         <v>0</v>
       </c>
     </row>
@@ -1776,7 +1523,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1788,7 +1535,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
rectifies an error in features.csv for Bant Spirit and adds an HEADER_PRESENT feature to magic.py
</commit_message>
<xml_diff>
--- a/BantSpirit/Training_set_BantSpirit/Features.xlsx
+++ b/BantSpirit/Training_set_BantSpirit/Features.xlsx
@@ -471,7 +471,7 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1146,13 +1146,13 @@
         <v>1</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -1184,13 +1184,13 @@
         <v>1</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -1398,7 +1398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>29</v>
       </c>

</xml_diff>